<commit_message>
set up for measure checking
</commit_message>
<xml_diff>
--- a/synquid/test/current/succinct/bfs_result.xlsb.xlsx
+++ b/synquid/test/current/succinct/bfs_result.xlsb.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="10050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="10050" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="succinct_vs_synquid" sheetId="1" r:id="rId1"/>
+    <sheet name="eager_typing_vs_synquid" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
   <si>
     <t>AVL-BalL0</t>
   </si>
@@ -249,6 +250,9 @@
   </si>
   <si>
     <t>List-Intersection</t>
+  </si>
+  <si>
+    <t>Eager</t>
   </si>
 </sst>
 </file>
@@ -359,7 +363,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>succinct_vs_synquid!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -380,7 +384,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$74</c:f>
+              <c:f>succinct_vs_synquid!$A$2:$A$74</c:f>
               <c:strCache>
                 <c:ptCount val="73"/>
                 <c:pt idx="0">
@@ -607,7 +611,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$74</c:f>
+              <c:f>succinct_vs_synquid!$B$2:$B$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="73"/>
@@ -838,7 +842,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>succinct_vs_synquid!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -859,7 +863,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$74</c:f>
+              <c:f>succinct_vs_synquid!$A$2:$A$74</c:f>
               <c:strCache>
                 <c:ptCount val="73"/>
                 <c:pt idx="0">
@@ -1086,7 +1090,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$74</c:f>
+              <c:f>succinct_vs_synquid!$C$2:$C$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="73"/>
@@ -1511,7 +1515,1258 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>eager_typing_vs_synquid!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eager</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>eager_typing_vs_synquid!$A$2:$A$75</c:f>
+              <c:strCache>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>AVL-BalL0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AVL-BalLL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVL-BalLR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AVL-BalR0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>AVL-BalRL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AVL-BalRR</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVL-Balance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AVL-Insert</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>AVL-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>AVL-Delete</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>RBT-BalanceL</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>RBT-BalanceR</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>RBT-Insert</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>List-Together</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Int-Max2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Int-Max3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Int-Max4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Int-Max5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Array-Search-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Array-Search-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Array-Search-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Array-Search-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Array-Search-6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Int-Add</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>List-Null</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>List-Elem</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>List-Stutter</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>List-Replicate</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>List-Append</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>List-Concat</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>List-Take</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>List-Drop</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>List-Delete</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>List-Map</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>List-ZipWith</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>List-Zip</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>List-ToNat</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>List-Product</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>List-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>List-Intersection</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>List-Fold</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>List-Fold-Length</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>List-Fold-Append</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>List-Ith</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>List-ElemIndex</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>List-Snoc</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>List-Reverse</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>UniqueList-Insert</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>UniqueList-Delete</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>UniqueList-Range</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>List-Nub</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>List-Compress</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>List-InsertSort</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>List-Fold-Sort</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>List-Split</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>IncList-Merge</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>IncList-MergeSort</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>List-Partition</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>IncList-PivotAppend</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>IncList-QuickSort</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Tree-Elem</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>Tree-Flatten</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>BST-Member</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>BST-Insert</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>BST-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>BST-Delete</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>BST-Sort</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>BinHeap-Member</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>BinHeap-Insert</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>Evaluator</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>AddressBook-Make</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>AddressBook-Merge</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>Replicate-Examples</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>eager_typing_vs_synquid!$B$2:$B$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="74"/>
+                <c:pt idx="0">
+                  <c:v>1.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8449999999999989</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.7650000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.44</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.78</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.405000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.265000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.58000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1749999999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.58499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.59000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.57499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.88500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.66500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.59499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.60499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.53500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.9350000000000005</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.86</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.65500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.59000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.55499999999999994</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.57499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.67500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.67999999999999994</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.81499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.7199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.55</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.3099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.2549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>20.075000000000003</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.1050000000000004</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.67500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.0700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>11.98</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>11.995000000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.83</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.41</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.15</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.5550000000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.115</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.57499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-48C5-40C7-8D8F-2FB7CE2428ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>eager_typing_vs_synquid!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Synquid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>eager_typing_vs_synquid!$A$2:$A$75</c:f>
+              <c:strCache>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>AVL-BalL0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AVL-BalLL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVL-BalLR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AVL-BalR0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>AVL-BalRL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AVL-BalRR</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVL-Balance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AVL-Insert</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>AVL-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>AVL-Delete</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>RBT-BalanceL</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>RBT-BalanceR</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>RBT-Insert</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>List-Together</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Int-Max2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Int-Max3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Int-Max4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Int-Max5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Array-Search-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Array-Search-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Array-Search-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Array-Search-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Array-Search-6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Int-Add</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>List-Null</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>List-Elem</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>List-Stutter</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>List-Replicate</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>List-Append</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>List-Concat</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>List-Take</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>List-Drop</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>List-Delete</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>List-Map</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>List-ZipWith</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>List-Zip</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>List-ToNat</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>List-Product</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>List-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>List-Intersection</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>List-Fold</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>List-Fold-Length</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>List-Fold-Append</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>List-Ith</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>List-ElemIndex</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>List-Snoc</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>List-Reverse</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>UniqueList-Insert</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>UniqueList-Delete</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>UniqueList-Range</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>List-Nub</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>List-Compress</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>List-InsertSort</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>List-Fold-Sort</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>List-Split</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>IncList-Merge</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>IncList-MergeSort</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>List-Partition</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>IncList-PivotAppend</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>IncList-QuickSort</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Tree-Elem</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>Tree-Flatten</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>BST-Member</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>BST-Insert</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>BST-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>BST-Delete</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>BST-Sort</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>BinHeap-Member</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>BinHeap-Insert</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>Evaluator</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>AddressBook-Make</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>AddressBook-Merge</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>Replicate-Examples</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>eager_typing_vs_synquid!$C$2:$C$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="74"/>
+                <c:pt idx="0">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.59</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55.38</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.29</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.57</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.1100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.36</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>7.53</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.04</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>21.1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.74</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>10.45</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-48C5-40C7-8D8F-2FB7CE2428ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="322520776"/>
+        <c:axId val="322527336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="322520776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="322527336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="322527336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="322520776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2054,6 +3309,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2075,6 +3833,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCA91B67-AECF-4465-A117-DCB7E4E5B24B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>22224</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>25399</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E670F7A3-E80F-4ACB-8A85-8FD8CECD9481}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2394,8 +4193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3209,4 +5008,828 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1.5299999999999998</v>
+      </c>
+      <c r="C2">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7.1099999999999994</v>
+      </c>
+      <c r="C3">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C4">
+        <v>9.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C5">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>8.2850000000000001</v>
+      </c>
+      <c r="C6">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>9.8449999999999989</v>
+      </c>
+      <c r="C7">
+        <v>9.5500000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3.0750000000000002</v>
+      </c>
+      <c r="C8">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>4.7650000000000006</v>
+      </c>
+      <c r="C9">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>6.0449999999999999</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>31.44</v>
+      </c>
+      <c r="C11">
+        <v>29.59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>33.78</v>
+      </c>
+      <c r="C12">
+        <v>32.19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>58.08</v>
+      </c>
+      <c r="C13">
+        <v>55.38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>19.405000000000001</v>
+      </c>
+      <c r="C14">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.51</v>
+      </c>
+      <c r="C16">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="C17">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1.19</v>
+      </c>
+      <c r="C18">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>10.265000000000001</v>
+      </c>
+      <c r="C19">
+        <v>8.17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="C20">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0.78</v>
+      </c>
+      <c r="C21">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>1.1749999999999998</v>
+      </c>
+      <c r="C22">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>2.3899999999999997</v>
+      </c>
+      <c r="C23">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C24">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.995</v>
+      </c>
+      <c r="C25">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0.59</v>
+      </c>
+      <c r="C26">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="C28">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="C29">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="C30">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0.625</v>
+      </c>
+      <c r="C31">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="C32">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="C33">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="C34">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="C35">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0.52</v>
+      </c>
+      <c r="C36">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0.53</v>
+      </c>
+      <c r="C37">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0.47</v>
+      </c>
+      <c r="C38">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39">
+        <v>1.6</v>
+      </c>
+      <c r="C39">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>6.9350000000000005</v>
+      </c>
+      <c r="C40">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41">
+        <v>5.86</v>
+      </c>
+      <c r="C41">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C42">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="C43">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>0.55499999999999994</v>
+      </c>
+      <c r="C44">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>0.54</v>
+      </c>
+      <c r="C45">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="C46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="C47">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="C48">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>0.76</v>
+      </c>
+      <c r="C49">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="C50">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="C51">
+        <v>4.1100000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>2.1</v>
+      </c>
+      <c r="C52">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>2.7199999999999998</v>
+      </c>
+      <c r="C53">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>1.22</v>
+      </c>
+      <c r="C54">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>3.55</v>
+      </c>
+      <c r="C55">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>2.3099999999999996</v>
+      </c>
+      <c r="C56">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>5.08</v>
+      </c>
+      <c r="C57">
+        <v>7.53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>4.2549999999999999</v>
+      </c>
+      <c r="C58">
+        <v>4.04</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59">
+        <v>20.075000000000003</v>
+      </c>
+      <c r="C59">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>1.06</v>
+      </c>
+      <c r="C60">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <v>5.1050000000000004</v>
+      </c>
+      <c r="C61">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>1.04</v>
+      </c>
+      <c r="C62">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>0.875</v>
+      </c>
+      <c r="C63">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="C64">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65">
+        <v>2.0700000000000003</v>
+      </c>
+      <c r="C65">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66">
+        <v>11.98</v>
+      </c>
+      <c r="C66">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>11.995000000000001</v>
+      </c>
+      <c r="C67">
+        <v>10.45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>2.83</v>
+      </c>
+      <c r="C68">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C69">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <v>1.41</v>
+      </c>
+      <c r="C70">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71">
+        <v>2.15</v>
+      </c>
+      <c r="C71">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72">
+        <v>1.5550000000000002</v>
+      </c>
+      <c r="C72">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73">
+        <v>1.115</v>
+      </c>
+      <c r="C73">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="C74">
+        <v>0.54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test cases for succinct
</commit_message>
<xml_diff>
--- a/synquid/test/current/succinct/bfs_result.xlsb.xlsx
+++ b/synquid/test/current/succinct/bfs_result.xlsb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="succinct_vs_synquid" sheetId="1" r:id="rId1"/>
@@ -4193,8 +4193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5014,7 +5014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>